<commit_message>
Improve identification if bookmark's chapter. Add some AppAward paperwork.
</commit_message>
<xml_diff>
--- a/doc/AppAward-MetadataTemplate.xlsx
+++ b/doc/AppAward-MetadataTemplate.xlsx
@@ -32,7 +32,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="103">
+  <si>
+    <t>Language Distribution</t>
+  </si>
+  <si>
+    <t>Theme</t>
+  </si>
+  <si>
+    <t>Wallpaper</t>
+  </si>
+  <si>
+    <t>Applications - Entertainment</t>
+  </si>
+  <si>
+    <t>Applications - Music</t>
+  </si>
+  <si>
+    <t>Applications - Photo &amp; Video</t>
+  </si>
+  <si>
+    <t>Applications - Sports</t>
+  </si>
+  <si>
+    <t>Applications - Social Networks</t>
+  </si>
+  <si>
+    <t>Games - Action</t>
+  </si>
+  <si>
+    <t>Games - Adventures</t>
+  </si>
+  <si>
+    <t>Games - Card &amp; Casino</t>
+  </si>
+  <si>
+    <t>Games - Education</t>
+  </si>
+  <si>
+    <t>Games - Puzzle</t>
+  </si>
+  <si>
+    <t>Games - Strategy</t>
+  </si>
+  <si>
+    <t>End Date for Published Content (Symbian and Java content cert expiry date)</t>
+  </si>
+  <si>
+    <t>Binary File Name (.Jad only)</t>
+  </si>
+  <si>
+    <t>AppUID (.sis only)</t>
+  </si>
+  <si>
+    <t>Symbian Signed Type (.sis only)</t>
+  </si>
+  <si>
+    <t>Symbian</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>WRT</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Flash</t>
+  </si>
+  <si>
+    <t>Symbian_Categories</t>
+  </si>
+  <si>
+    <t>Java_Categories</t>
+  </si>
+  <si>
+    <t>WRT_Categories</t>
+  </si>
+  <si>
+    <t>Audio_Categories</t>
+  </si>
+  <si>
+    <t>Video_Categories</t>
+  </si>
+  <si>
+    <t>Theme_Categories</t>
+  </si>
+  <si>
+    <t>dorian-256.png</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
   <si>
     <t>Wallpaper_Categories</t>
   </si>
@@ -257,96 +351,6 @@
   </si>
   <si>
     <t>Country Distribution</t>
-  </si>
-  <si>
-    <t>Language Distribution</t>
-  </si>
-  <si>
-    <t>Theme</t>
-  </si>
-  <si>
-    <t>Wallpaper</t>
-  </si>
-  <si>
-    <t>Applications - Entertainment</t>
-  </si>
-  <si>
-    <t>Applications - Music</t>
-  </si>
-  <si>
-    <t>Applications - Photo &amp; Video</t>
-  </si>
-  <si>
-    <t>Applications - Sports</t>
-  </si>
-  <si>
-    <t>Applications - Social Networks</t>
-  </si>
-  <si>
-    <t>Games - Action</t>
-  </si>
-  <si>
-    <t>Games - Adventures</t>
-  </si>
-  <si>
-    <t>Games - Card &amp; Casino</t>
-  </si>
-  <si>
-    <t>Games - Education</t>
-  </si>
-  <si>
-    <t>Games - Puzzle</t>
-  </si>
-  <si>
-    <t>Games - Strategy</t>
-  </si>
-  <si>
-    <t>End Date for Published Content (Symbian and Java content cert expiry date)</t>
-  </si>
-  <si>
-    <t>Binary File Name (.Jad only)</t>
-  </si>
-  <si>
-    <t>AppUID (.sis only)</t>
-  </si>
-  <si>
-    <t>Symbian Signed Type (.sis only)</t>
-  </si>
-  <si>
-    <t>Symbian</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>WRT</t>
-  </si>
-  <si>
-    <t>Audio</t>
-  </si>
-  <si>
-    <t>Video</t>
-  </si>
-  <si>
-    <t>Flash</t>
-  </si>
-  <si>
-    <t>Symbian_Categories</t>
-  </si>
-  <si>
-    <t>Java_Categories</t>
-  </si>
-  <si>
-    <t>WRT_Categories</t>
-  </si>
-  <si>
-    <t>Audio_Categories</t>
-  </si>
-  <si>
-    <t>Video_Categories</t>
-  </si>
-  <si>
-    <t>Theme_Categories</t>
   </si>
 </sst>
 </file>
@@ -778,8 +782,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Z1050"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="L1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -815,119 +819,121 @@
   <sheetData>
     <row r="1" spans="1:26" s="6" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="W1" s="5" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>72</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="22">
       <c r="A2" s="7" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="L2" s="1"/>
       <c r="M2" s="9" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="4"/>
@@ -937,20 +943,20 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="V2" s="1"/>
       <c r="W2" s="8" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -6479,532 +6485,532 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="5" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>98</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="O1" t="s">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="P1" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="Q1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="I2" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="L2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="M2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" t="s">
         <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="I3" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="R3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="I4" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="N4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="O4" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="R4" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="I5" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="K5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="L5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="N5" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="O5" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="R5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="I6" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="N6" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="R6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="I7" t="s">
-        <v>73</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="R7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="I8" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="L8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="M8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="N8" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="O8" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="R8" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="I9" t="s">
-        <v>95</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="M9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="N9" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="O9" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="R9" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="I10" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="K10" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="L10" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="M10" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="R10" t="s">
-        <v>76</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="J11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="K11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="L11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="M11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="R11" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="J12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="L12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="M12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="R12" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="J13" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="L13" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="M13" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="R13" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="J14" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="K14" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="L14" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="M14" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="R14" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="J15" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="K15" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="L15" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="M15" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
       <c r="R15" t="s">
-        <v>78</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="J16" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="K16" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="L16" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="M16" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="R16" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="10:18">
       <c r="J17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="K17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="L17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="M17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="R17" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="10:18">
       <c r="J18" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="L18" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="M18" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="R18" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="10:18">
       <c r="J19" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="M19" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="R19" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="10:18">
       <c r="J20" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="K20" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="L20" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="M20" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="R20" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="10:18">
       <c r="J21" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="K21" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="L21" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="M21" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
       <c r="R21" t="s">
-        <v>83</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="10:18">
       <c r="J22" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="L22" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="M22" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
       <c r="R22" t="s">
-        <v>84</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="10:18">
       <c r="J23" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="K23" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="L23" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="M23" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="R23" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="10:18">
       <c r="J24" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="L24" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="M24" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="R24" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="10:18">
       <c r="J25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="L25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="M25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="R25" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>